<commit_message>
Heating technology costs: documentation of cost functions and calculation methodology of FORECAST in data_prep. Scenario table for labor input of heating technology installation and parameter tables for parameters of cost functions in input are added.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_HeatingTechnology_Cost_Material.xlsx
+++ b/projects/test_building/input/Parameter_HeatingTechnology_Cost_Material.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1665" windowWidth="19860" windowHeight="13515"/>
+    <workbookView xWindow="1500" yWindow="1670" windowWidth="17700" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="13">
   <si>
     <t>id_region</t>
   </si>
@@ -34,25 +34,40 @@
     <t>id_heating_system_action</t>
   </si>
   <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>learning_effect</t>
+    <t>multiplier_cost</t>
+  </si>
+  <si>
+    <t>exponent_cost</t>
+  </si>
+  <si>
+    <t>multiplier_share</t>
+  </si>
+  <si>
+    <t>exponent_share</t>
+  </si>
+  <si>
+    <t>learning_effect (cagr)</t>
+  </si>
+  <si>
+    <t>PP_index</t>
+  </si>
+  <si>
+    <t>wages_index</t>
+  </si>
+  <si>
+    <t>criterion_small</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,10 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,17 +171,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H76" totalsRowShown="0">
-  <autoFilter ref="A1:H76"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L76" totalsRowShown="0">
+  <autoFilter ref="A1:L76"/>
+  <tableColumns count="12">
     <tableColumn id="2" name="id_region"/>
     <tableColumn id="4" name="id_heating_technology" dataDxfId="0"/>
     <tableColumn id="5" name="id_heating_system_action"/>
     <tableColumn id="6" name="unit"/>
-    <tableColumn id="7" name="2010"/>
-    <tableColumn id="8" name="2011"/>
-    <tableColumn id="1" name="2012"/>
-    <tableColumn id="3" name="learning_effect"/>
+    <tableColumn id="7" name="multiplier_cost"/>
+    <tableColumn id="8" name="exponent_cost"/>
+    <tableColumn id="1" name="multiplier_share"/>
+    <tableColumn id="9" name="exponent_share"/>
+    <tableColumn id="10" name="criterion_small"/>
+    <tableColumn id="3" name="learning_effect (cagr)"/>
+    <tableColumn id="11" name="PP_index"/>
+    <tableColumn id="12" name="wages_index"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -433,23 +454,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,19 +490,31 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>9</v>
       </c>
@@ -486,22 +525,34 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>17477</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>-0.69899999999999995</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.16919999999999999</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L2">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
@@ -512,22 +563,34 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>7866.3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>-0.70499999999999996</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.33169999999999999</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7.8399999999999997E-2</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L3">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>9</v>
       </c>
@@ -538,22 +601,34 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>5172.3999999999996</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>-0.32900000000000001</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.23330000000000001</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L4">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>9</v>
       </c>
@@ -564,22 +639,34 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>8463.2900000000009</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.42437999999999998</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L5">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>9</v>
       </c>
@@ -590,22 +677,34 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2572.02</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.69674000000000003</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L6">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9</v>
       </c>
@@ -616,22 +715,34 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>9382.89</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.49456</v>
       </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L7">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9</v>
       </c>
@@ -642,22 +753,34 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>8877</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0.38796999999999998</v>
       </c>
       <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L8">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -668,22 +791,34 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>5973.77</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0.64493</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L9">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -694,22 +829,34 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>9842.25</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0.46034999999999998</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L10">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -720,22 +867,34 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>7293.99</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>-0.38200000000000001</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0.59730000000000005</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.128</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L11">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -746,22 +905,34 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>5534.54</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>-0.35</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0.60565999999999998</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.11700000000000001</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L12">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>9</v>
       </c>
@@ -772,22 +943,34 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>7869.84</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>-0.38500000000000001</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.114</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L13">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9</v>
       </c>
@@ -798,22 +981,34 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>7693.9</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.38579999999999998</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L14">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>9</v>
       </c>
@@ -824,22 +1019,34 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2338.1999999999998</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L15">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9</v>
       </c>
@@ -850,22 +1057,34 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>8529.9</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0.4496</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L16">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>9</v>
       </c>
@@ -876,22 +1095,34 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>12105</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0.52905000000000002</v>
       </c>
       <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L17">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -902,22 +1133,34 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>8146.05</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0.87944999999999995</v>
       </c>
       <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L18">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9</v>
       </c>
@@ -928,22 +1171,34 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>13421.25</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.62775000000000003</v>
       </c>
       <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L19">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>9</v>
       </c>
@@ -954,22 +1209,34 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>19234.75</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0.96450000000000002</v>
       </c>
       <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L20">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9</v>
       </c>
@@ -980,22 +1247,34 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>5845.5</v>
       </c>
       <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
+        <v>-0.37</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1.5834999999999999</v>
       </c>
       <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L21">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1006,22 +1285,34 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>21324.75</v>
       </c>
       <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1.1240000000000001</v>
       </c>
       <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L22">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1032,22 +1323,34 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>20175</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0.88175000000000003</v>
       </c>
       <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L23">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1058,22 +1361,34 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>13576.75</v>
       </c>
       <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1.4657500000000001</v>
       </c>
       <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L24">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1084,22 +1399,34 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>22368.75</v>
       </c>
       <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.0462499999999999</v>
       </c>
       <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L25">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1110,22 +1437,34 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>16577.25</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
+        <v>-0.38200000000000001</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.3574999999999999</v>
       </c>
       <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.128</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L26">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1136,22 +1475,34 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>12578.5</v>
       </c>
       <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
+        <v>-0.35</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1.3765000000000001</v>
       </c>
       <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.11700000000000001</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L27">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1162,22 +1513,34 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>17886</v>
       </c>
       <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
+        <v>-0.38500000000000001</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1.4375</v>
       </c>
       <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.114</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L28">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1188,22 +1551,34 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>3684.2</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0.44119999999999998</v>
       </c>
       <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K29">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L29">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1214,22 +1589,34 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2563.9</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0.61229999999999996</v>
       </c>
       <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K30">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L30">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>9</v>
       </c>
@@ -1240,22 +1627,34 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>4036.4</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K31">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L31">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1266,22 +1665,34 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>4775.7</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>-0.19</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0.40060000000000001</v>
       </c>
       <c r="H32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K32">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L32">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1292,22 +1703,34 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>3447.4</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>-0.21299999999999999</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0.76480000000000004</v>
       </c>
       <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-7.6999999999999999E-2</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K33">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L33">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1318,22 +1741,34 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>5211</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>-0.192</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0.74480000000000002</v>
       </c>
       <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.5999999999999993E-2</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K34">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L34">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>9</v>
       </c>
@@ -1344,22 +1779,34 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>4775.7</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>-0.19</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0.40060000000000001</v>
       </c>
       <c r="H35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-9.4E-2</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K35">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L35">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1370,22 +1817,34 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>3447.4</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>-0.21299999999999999</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0.76480000000000004</v>
       </c>
       <c r="H36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-7.6999999999999999E-2</v>
+      </c>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K36">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L36">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>9</v>
       </c>
@@ -1396,22 +1855,34 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>5211</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>-0.192</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0.74480000000000002</v>
       </c>
       <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.5999999999999993E-2</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K37">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L37">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1422,22 +1893,34 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>1842.1</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0.22059999999999999</v>
       </c>
       <c r="H38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L38">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9</v>
       </c>
@@ -1448,22 +1931,34 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>1281.95</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0.30614999999999998</v>
       </c>
       <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L39">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>9</v>
       </c>
@@ -1474,22 +1969,34 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>2018.2</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0.246</v>
       </c>
       <c r="H40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L40">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>9</v>
       </c>
@@ -1500,22 +2007,34 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>9617.375</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0.38579999999999998</v>
       </c>
       <c r="H41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I41">
+        <v>10</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L41">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>9</v>
       </c>
@@ -1526,22 +2045,34 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2922.75</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L42">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>9</v>
       </c>
@@ -1552,22 +2083,34 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E43" s="3">
+        <v>10662.375</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0.4496</v>
       </c>
       <c r="H43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L43">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>9</v>
       </c>
@@ -1578,22 +2121,34 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>7693.9</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0.38579999999999998</v>
       </c>
       <c r="H44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L44">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>9</v>
       </c>
@@ -1604,22 +2159,34 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>2338.1999999999998</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="H45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I45">
+        <v>10</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L45">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>9</v>
       </c>
@@ -1630,22 +2197,34 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>8529.9</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0.4496</v>
       </c>
       <c r="H46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L46">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>9</v>
       </c>
@@ -1656,22 +2235,34 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>8070</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0.35270000000000001</v>
       </c>
       <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L47">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>9</v>
       </c>
@@ -1682,22 +2273,34 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>5430.7</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>0.58630000000000004</v>
       </c>
       <c r="H48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L48">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>9</v>
       </c>
@@ -1708,22 +2311,34 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>8947.5</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0.41849999999999998</v>
       </c>
       <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I49">
+        <v>10</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L49">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>9</v>
       </c>
@@ -1734,22 +2349,34 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>3684.2</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0.44119999999999998</v>
       </c>
       <c r="H50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K50">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L50">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>9</v>
       </c>
@@ -1760,22 +2387,34 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>2563.9</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0.61229999999999996</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="I51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K51">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L51">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>9</v>
       </c>
@@ -1786,22 +2425,34 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>4036.4</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="H52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="K52">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L52">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>9</v>
       </c>
@@ -1812,22 +2463,34 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>1842.1</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0.22059999999999999</v>
       </c>
       <c r="H53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L53">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9</v>
       </c>
@@ -1838,22 +2501,34 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>1281.95</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0.30614999999999998</v>
       </c>
       <c r="H54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L54">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>9</v>
       </c>
@@ -1864,22 +2539,34 @@
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>2018.2</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0.246</v>
       </c>
       <c r="H55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L55">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>9</v>
       </c>
@@ -1890,22 +2577,34 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>7693.9</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0.38579999999999998</v>
       </c>
       <c r="H56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I56">
+        <v>10</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L56">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>9</v>
       </c>
@@ -1916,22 +2615,34 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>2338.1999999999998</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="H57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L57">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>9</v>
       </c>
@@ -1942,22 +2653,34 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>8529.9</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0.4496</v>
       </c>
       <c r="H58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I58">
+        <v>10</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L58">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>9</v>
       </c>
@@ -1968,22 +2691,34 @@
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>8070</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0.35270000000000001</v>
       </c>
       <c r="H59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L59">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>9</v>
       </c>
@@ -1994,22 +2729,34 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>5430.7</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0.58630000000000004</v>
       </c>
       <c r="H60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L60">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>9</v>
       </c>
@@ -2020,22 +2767,34 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>8947.5</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0.41849999999999998</v>
       </c>
       <c r="H61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L61">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>9</v>
       </c>
@@ -2046,22 +2805,34 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>6630.9</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>-0.38200000000000001</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.128</v>
+      </c>
+      <c r="I62">
+        <v>10</v>
+      </c>
+      <c r="J62">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K62">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L62">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>9</v>
       </c>
@@ -2072,22 +2843,34 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>5031.3999999999996</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>-0.35</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0.55059999999999998</v>
       </c>
       <c r="H63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.11700000000000001</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+      <c r="J63">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K63">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L63">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>9</v>
       </c>
@@ -2098,22 +2881,34 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>7154.4</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>-0.38500000000000001</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="H64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.114</v>
+      </c>
+      <c r="I64">
+        <v>10</v>
+      </c>
+      <c r="J64">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K64">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L64">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>9</v>
       </c>
@@ -2124,22 +2919,34 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>7693.9</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>-0.53</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>0.38579999999999998</v>
       </c>
       <c r="H65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I65">
+        <v>10</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L65">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>9</v>
       </c>
@@ -2150,22 +2957,34 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>2338.1999999999998</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>-0.37</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0.63339999999999996</v>
       </c>
       <c r="H66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.105</v>
+      </c>
+      <c r="I66">
+        <v>10</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L66">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>9</v>
       </c>
@@ -2176,22 +2995,34 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>8529.9</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0.4496</v>
       </c>
       <c r="H67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="I67">
+        <v>10</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L67">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -2202,22 +3033,34 @@
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>12105</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>-0.56200000000000006</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0.52905000000000002</v>
       </c>
       <c r="H68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="I68">
+        <v>10</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L68">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>9</v>
       </c>
@@ -2228,22 +3071,34 @@
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>8146.05</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>-0.52500000000000002</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0.87944999999999995</v>
       </c>
       <c r="H69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L69">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>9</v>
       </c>
@@ -2254,22 +3109,34 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>13421.25</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>-0.56899999999999995</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0.62775000000000003</v>
       </c>
       <c r="H70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I70">
+        <v>10</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L70">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>9</v>
       </c>
@@ -2280,22 +3147,34 @@
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>1842.1</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0.22059999999999999</v>
       </c>
       <c r="H71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L71">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>9</v>
       </c>
@@ -2306,22 +3185,34 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>1281.95</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0.30614999999999998</v>
       </c>
       <c r="H72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.6999999999999994E-2</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L72">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>9</v>
       </c>
@@ -2332,22 +3223,34 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>2018.2</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0.246</v>
       </c>
       <c r="H73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L73">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>9</v>
       </c>
@@ -2358,22 +3261,34 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>8246.9</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>-0.29899999999999999</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0.34520000000000001</v>
       </c>
       <c r="H74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+      <c r="I74">
+        <v>5</v>
+      </c>
+      <c r="J74">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K74">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L74">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>9</v>
       </c>
@@ -2384,22 +3299,34 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>4663.6000000000004</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>-0.25700000000000001</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0.76329999999999998</v>
       </c>
       <c r="H75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-0.156</v>
+      </c>
+      <c r="I75">
+        <v>5</v>
+      </c>
+      <c r="J75">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K75">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L75">
+        <v>0.67706708268330695</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>9</v>
       </c>
@@ -2410,19 +3337,31 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>10345</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>-0.32900000000000001</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0.50209999999999999</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>-0.11600000000000001</v>
+      </c>
+      <c r="I76">
+        <v>5</v>
+      </c>
+      <c r="J76">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K76">
+        <v>0.74868004223864804</v>
+      </c>
+      <c r="L76">
+        <v>0.67706708268330695</v>
       </c>
     </row>
   </sheetData>
@@ -2441,379 +3380,379 @@
       <selection activeCell="C78" sqref="C4:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C10">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C12">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C14">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C15">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C16">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34">
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35">
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36">
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37">
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38">
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39">
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40">
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41">
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43">
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44">
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45">
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65">
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66">
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67">
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72">
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73">
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75">
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76">
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77">
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78">
         <v>50</v>
       </c>

</xml_diff>